<commit_message>
Ditto Pachen - EFT Changes
</commit_message>
<xml_diff>
--- a/Development/Artifacts/Changes From 05 May.xlsx
+++ b/Development/Artifacts/Changes From 05 May.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Bugzilla Ticket No</t>
   </si>
@@ -41,6 +41,39 @@
   </si>
   <si>
     <t>How is done by Developer (Explain in detail)</t>
+  </si>
+  <si>
+    <t>EFT Changes. Façade, Service Layer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREATE TABLE MOLSAEFTUSERCONFIGURATION(CONFIGURATIONID BIGINT not null, USERNAME1 CHARACTER(64), USERNAME2 CHARACTER(64), 
+USERTITLE1 CHARACTER(100), USERTITLE2 CHARACTER(100), EFFECTIVEDATETIME DATE, RECORDSTATUS CHARACTER(10), VERSIONNO INT not null, LASTWRITTEN DATE);
+ALTER TABLE MOLSAEFTUSERCONFIGURATION ADD CONSTRAINT MOLSAEFTUSERCONFIGURATION PRIMARY KEY(CONFIGURATIONID);
+INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSAEFTUserConfiguration.configureUsersForEFTLetterConfiguration', 'curam', 'molsa.eft.eftletter.facade', 'curam.molsa.eft.eftletter.facade.MOLSAEFTUserConfiguration.configureUsersForEFTLetterConfiguration', 'Y');
+INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSAEFTUserConfiguration.listAllUsersByPosition', 'curam', 'molsa.eft.eftletter.facade', 'curam.molsa.eft.eftletter.facade.MOLSAEFTUserConfiguration.listAllUsersByPosition', 'Y');
+INSERT INTO FunctionIdentifier (fidName, projectPackage, codePackage, description, fidEnabled) values ('MOLSAEFTUserConfiguration.listUsersConfiguredForEFTLetter', 'curam', 'molsa.eft.eftletter.facade', 'curam.molsa.eft.eftletter.facade.MOLSAEFTUserConfiguration.listUsersConfiguredForEFTLetter', 'Y');
+INSERT INTO SECURITYIDENTIFIER (DESCRIPTION, LASTWRITTEN, SIDNAME, SIDTYPE, VERSIONNO) VALUES (null, '2015-03-03 03:42:25', 'MOLSAEFTUserConfiguration.configureUsersForEFTLetterConfiguration', 'FUNCTION', 0);
+INSERT INTO SECURITYIDENTIFIER (DESCRIPTION, LASTWRITTEN, SIDNAME, SIDTYPE, VERSIONNO) VALUES (null, '2015-03-03 03:42:25', 'MOLSAEFTUserConfiguration.listAllUsersByPosition', 'FUNCTION', 0);
+INSERT INTO SECURITYIDENTIFIER (DESCRIPTION, LASTWRITTEN, SIDNAME, SIDTYPE, VERSIONNO) VALUES (null, '2015-03-03 03:42:25', 'MOLSAEFTUserConfiguration.listUsersConfiguredForEFTLetter', 'FUNCTION', 0);
+INSERT INTO SECURITYFIDSID(SIDNAME, FIDNAME, LASTWRITTEN) VALUES ('MOLSAEFTUserConfiguration.configureUsersForEFTLetterConfiguration','MOLSAEFTUserConfiguration.configureUsersForEFTLetterConfiguration');
+INSERT INTO SECURITYFIDSID(SIDNAME, FIDNAME, LASTWRITTEN) VALUES ('MOLSAEFTUserConfiguration.listAllUsersByPosition','MOLSAEFTUserConfiguration.listAllUsersByPosition');
+INSERT INTO SECURITYFIDSID(SIDNAME, FIDNAME, LASTWRITTEN) VALUES('MOLSAEFTUserConfiguration.listUsersConfiguredForEFTLetter','MOLSAEFTUserConfiguration.listUsersConfiguredForEFTLetter');
+INSERT INTO SECURITYGROUPSID (GROUPNAME, LASTWRITTEN, SIDNAME) VALUES ('SUPERGROUP', null, 'MOLSAEFTUserConfiguration.configureUsersForEFTLetterConfiguration');
+INSERT INTO SECURITYGROUPSID (GROUPNAME, LASTWRITTEN, SIDNAME) VALUES ('SUPERGROUP', null, 'MOLSAEFTUserConfiguration.listAllUsersByPosition');
+INSERT INTO SECURITYGROUPSID (GROUPNAME, LASTWRITTEN, SIDNAME) VALUES ('SUPERGROUP', null, 'MOLSAEFTUserConfiguration.listUsersConfiguredForEFTLetter');
+--Manger job Update
+update job set NAME='مدير ادارة الضمان الاجتماعي' , comments='مدير ادارة الضمان الاجتماعي' where jobid=45014;
+--Need to update Assistance Manager Job
+INSERT INTO JOB (COMMENTS, JOBID, NAME, RECORDSTATUS, VERSIONNO) VALUES ('Assistance manager', 45021, 'Assistance manager', 'RST1', 1);
+update POSITION  set jobid=45021 where positionid=45290;
+--New Job for General Secrartey وكيل الوزارة المساعد للشؤون الاجتماعية
+INSERT INTO JOB (COMMENTS, JOBID, NAME, RECORDSTATUS, VERSIONNO) VALUES ('General  Secretary', 45020, 'General Secretary', 'RST1', 1);
+INSERT INTO POSITION (COMMENTS, FROMDATE, JOBID, LASTWRITTEN, LEADPOSITIONIND, NAME, POSITIONID, RECORDSTATUS, TODATE, VERSIONNO) VALUES ('General Secretary', '2003-01-01', 45020, '2006-01-01 00:00:00', '0', 'General Secretary', 45349, 'RST1', null, 1);
+INSERT INTO ORGUNITPOSITIONLINK (ORGUNITPOSITIONLINKID, ORGANISATIONUNITID, POSITIONID, ORGANISATIONSTRUCTUREID, RECORDSTATUS, VERSIONNO) VALUES (45356, 45002, 45349,45000, 'RST1', 1);
+</t>
+  </si>
+  <si>
+    <t>Harisha</t>
   </si>
 </sst>
 </file>
@@ -427,9 +460,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:I4"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,7 +471,7 @@
     <col min="3" max="3" width="72.42578125" customWidth="1"/>
     <col min="4" max="4" width="35.42578125" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="39.140625" customWidth="1"/>
+    <col min="7" max="7" width="187.85546875" customWidth="1"/>
     <col min="8" max="8" width="12.140625" customWidth="1"/>
     <col min="9" max="9" width="53.140625" customWidth="1"/>
   </cols>
@@ -472,9 +505,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C2" s="1"/>
-      <c r="G2" s="1"/>
+    <row r="2" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -510,65 +550,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003520CC91E1C90A4F9689A135D663C63F" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5bea9beecb72e899f05172e22af69af0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e967487d-3eea-483d-b969-e50e6c114ffa" xmlns:ns3="43475cab-d89f-451e-a1e3-4db005e0f558" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="438d5435a0413bb8242127eebe6f163c" ns2:_="" ns3:_="">
     <xsd:import namespace="e967487d-3eea-483d-b969-e50e6c114ffa"/>
@@ -752,6 +733,65 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -772,22 +812,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A3CD956-F256-4860-8B56-AE881D5ADEC8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6F0B25-6AD0-4AF9-AE4F-0D8285608470}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0051AA5-43D6-41A0-9086-D5D3DFF72221}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -806,6 +830,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6F0B25-6AD0-4AF9-AE4F-0D8285608470}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A3CD956-F256-4860-8B56-AE881D5ADEC8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1926F8BC-3749-487B-86BA-515B8CAD861D}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Joseph  - Training Changes
</commit_message>
<xml_diff>
--- a/Development/Artifacts/Changes From 05 May.xlsx
+++ b/Development/Artifacts/Changes From 05 May.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Bugzilla Ticket No</t>
   </si>
@@ -74,6 +74,15 @@
   </si>
   <si>
     <t>Harisha</t>
+  </si>
+  <si>
+    <t>Joseph</t>
+  </si>
+  <si>
+    <t>Use inserttabconfifuration</t>
+  </si>
+  <si>
+    <t>Changes to Navigation Files - Service Offering.nav files</t>
   </si>
 </sst>
 </file>
@@ -460,9 +469,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +527,15 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -550,6 +567,65 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003520CC91E1C90A4F9689A135D663C63F" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5bea9beecb72e899f05172e22af69af0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e967487d-3eea-483d-b969-e50e6c114ffa" xmlns:ns3="43475cab-d89f-451e-a1e3-4db005e0f558" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="438d5435a0413bb8242127eebe6f163c" ns2:_="" ns3:_="">
     <xsd:import namespace="e967487d-3eea-483d-b969-e50e6c114ffa"/>
@@ -733,65 +809,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -812,6 +829,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A3CD956-F256-4860-8B56-AE881D5ADEC8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6F0B25-6AD0-4AF9-AE4F-0D8285608470}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0051AA5-43D6-41A0-9086-D5D3DFF72221}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -830,22 +863,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6F0B25-6AD0-4AF9-AE4F-0D8285608470}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A3CD956-F256-4860-8B56-AE881D5ADEC8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1926F8BC-3749-487B-86BA-515B8CAD861D}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Added entries. - Smitha
</commit_message>
<xml_diff>
--- a/Development/Artifacts/Changes From 05 May.xlsx
+++ b/Development/Artifacts/Changes From 05 May.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Bugzilla Ticket No</t>
   </si>
@@ -123,6 +123,50 @@
   </si>
   <si>
     <t>build creole.upload.rulesets</t>
+  </si>
+  <si>
+    <t>EJBServer/components/MOLSACP/source/curam/molsacp/impl/Module.java
+EJBServer/components/MOLSACP/source/curam/molsacp/impl/MOLSAScreeningHelper.java
+EJBServer/components/MOLSACP/source/curam/molsacp/eventlisteners/impl/MOLSAScreeningEventListener.java
+EJBServer/components/MOLSACP/model/Packages/Screening/Screening.efx
+EJBServer/components/MOLSACP/model/Packages/Domain Definition/Domain Definition.efx
+EJBServer/components/MOLSACP/data/initial/ModuleClassName.dmx</t>
+  </si>
+  <si>
+    <t>INSERT INTO MODULECLASSNAME (MODULECLASSNAME) VALUES ('curam.molsacp.impl.Module');
+CREATE TABLE MOLSASCREENINGINFO(
+SCREENINGINFOID BIGINT not null, 
+QID CHARACTER(18), 
+GENDER CHARACTER(10), 
+NAME CHARACTER(131), 
+DATEOFBIRTH DATE, 
+MARITALSTATUS CHARACTER(10), 
+QATARI CHARACTER(1) not null, 
+RESIDENT CHARACTER(1) not null, 
+SCHOOLENROLLED CHARACTER(1) not null, 
+PHONENUMBER CHARACTER(40), 
+ABSENTFATHER CHARACTER(1) not null, 
+UNKNOWNPARENT CHARACTER(1) not null, 
+HANDICAP CHARACTER(1) not null, 
+UNABLETOWORK CHARACTER(1) not null, 
+MAIDALLOWANCE CHARACTER(1) not null, 
+RELATEDID BIGINT, 
+VERSIONNO INT not null, 
+LASTWRITTEN TIMESTAMP
+);
+CREATE TABLE MOLSASCREENINGINCOMEINFO(
+SCREENINGINCOMEINFOID BIGINT not null, 
+SCREENINGINFOID BIGINT, 
+INCOMETYPE CHARACTER(10), 
+AMOUNT DECIMAL(31,2) not null, 
+FREQUENCY CHARACTER(10), 
+VERSIONNO INT not null, 
+LASTWRITTEN TIMESTAMP
+);
+ALTER TABLE MOLSASCREENINGINFO ADD
+CONSTRAINT MOLSASCREENINGINFO PRIMARY KEY(SCREENINGINFOID);
+ALTER TABLE MOLSASCREENINGINCOMEINFO ADD
+CONSTRAINT MOLSASCREENINGINCOMEINFO PRIMARY KEY(SCREENINGINCOMEINFOID);</t>
   </si>
 </sst>
 </file>
@@ -507,11 +551,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,6 +676,23 @@
       <c r="G7" s="1"/>
       <c r="I7" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>382</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added related to Application timer - Smitha
</commit_message>
<xml_diff>
--- a/Development/Artifacts/Changes From 05 May.xlsx
+++ b/Development/Artifacts/Changes From 05 May.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Bugzilla Ticket No</t>
   </si>
@@ -167,6 +167,22 @@
 CONSTRAINT MOLSASCREENINGINFO PRIMARY KEY(SCREENINGINFOID);
 ALTER TABLE MOLSASCREENINGINCOMEINFO ADD
 CONSTRAINT MOLSASCREENINGINCOMEINFO PRIMARY KEY(SCREENINGINCOMEINFOID);</t>
+  </si>
+  <si>
+    <t>EJBServer\components\MOLSA_ar\data\initial\WORKQUEUE.dmx
+EJBServer\components\MOLSA_ar\codetable\CT_ProgramWithdrawalRequestReason.ctx
+EJBServer\components\MOLSA\message\MOLSANotification.xml
+EJBServer\components\MOLSA\codetable\CT_ProgramWithdrawalRequestReason.ctx
+EJBServer\components\MOLSA\data\initial\clob\MOLSAIntakeConfiguration.xml
+EJBServer\components\MOLSA\data\initial\ALLOCATIONTARGET.dmx
+EJBServer\components\MOLSA\data\initial\ALLOCATIONTARGETITEM.dmx
+EJBServer\components\MOLSA\data\initial\MILESTONECONFIGURATION.dmx
+EJBServer\components\MOLSA\data\initial\WORKQUEUE.dmx
+EJBServer\components\MOLSA\events\handler_config.xml
+EJBServer\components\MOLSA\source\curam\molsa\constants\impl\MOLSAConstants.java
+EJBServer\components\MOLSA\source\curam\molsa\creoleprogramrecommendation\sl\event\impl\MOLSAApplicationDenialHandler.java
+EJBServer\components\MOLSA\source\curam\molsa\creoleprogramrecommendation\sl\event\impl\MolsaStatusChangedHandler.java
+EJBServer\components\MOLSA\workflow\MOLSAApplicationWithdrawTask_v1.xml</t>
   </si>
 </sst>
 </file>
@@ -551,11 +567,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,6 +711,17 @@
         <v>24</v>
       </c>
     </row>
+    <row r="9" spans="1:9" ht="240" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
@@ -707,84 +734,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">UQKZYU5EZKJQ-17-950</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
-      <Url>https://dionatec.sharepoint.com/GlobalServices/_layouts/15/DocIdRedir.aspx?ID=UQKZYU5EZKJQ-17-950</Url>
-      <Description>UQKZYU5EZKJQ-17-950</Description>
-    </_dlc_DocIdUrl>
-    <SharedWithUsers xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003520CC91E1C90A4F9689A135D663C63F" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5bea9beecb72e899f05172e22af69af0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e967487d-3eea-483d-b969-e50e6c114ffa" xmlns:ns3="43475cab-d89f-451e-a1e3-4db005e0f558" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="438d5435a0413bb8242127eebe6f163c" ns2:_="" ns3:_="">
     <xsd:import namespace="e967487d-3eea-483d-b969-e50e6c114ffa"/>
@@ -968,40 +917,85 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">UQKZYU5EZKJQ-17-950</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
+      <Url>https://dionatec.sharepoint.com/GlobalServices/_layouts/15/DocIdRedir.aspx?ID=UQKZYU5EZKJQ-17-950</Url>
+      <Description>UQKZYU5EZKJQ-17-950</Description>
+    </_dlc_DocIdUrl>
+    <SharedWithUsers xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1926F8BC-3749-487B-86BA-515B8CAD861D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="e967487d-3eea-483d-b969-e50e6c114ffa"/>
-    <ds:schemaRef ds:uri="43475cab-d89f-451e-a1e3-4db005e0f558"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A3CD956-F256-4860-8B56-AE881D5ADEC8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6F0B25-6AD0-4AF9-AE4F-0D8285608470}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0051AA5-43D6-41A0-9086-D5D3DFF72221}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1018,4 +1012,37 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6F0B25-6AD0-4AF9-AE4F-0D8285608470}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A3CD956-F256-4860-8B56-AE881D5ADEC8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1926F8BC-3749-487B-86BA-515B8CAD861D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e967487d-3eea-483d-b969-e50e6c114ffa"/>
+    <ds:schemaRef ds:uri="43475cab-d89f-451e-a1e3-4db005e0f558"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>